<commit_message>
Eliminar archivos de respaldo y actualizar dependencias en requirements.txt
</commit_message>
<xml_diff>
--- a/REVs/REV-08-05-2025.xlsx
+++ b/REVs/REV-08-05-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R74"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3813,20 +3813,726 @@
           <t>ML</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
         </is>
       </c>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
-      <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr"/>
-      <c r="P74" t="inlineStr"/>
-      <c r="Q74" t="inlineStr"/>
-      <c r="R74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>6XS17353</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>TOPICREM CREMA CALMANTE 40ML</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>6XS18000</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>TOPICREM BABY 2EN1 GEL LIMPIADOR 500ML</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2CC05367</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>KRISTIN THE ONE PURPLE SHAMPOO 296 ML</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>CABELLO ACONDIC. SUAVIZANTE</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>296</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>4EF05522</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>BENCH TOGETHER SET HER 30 ML+75ML SG</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>PERF. ESTUCHES MUJER</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>4EM03368</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>BENCH TOGETHER SET HIM 30 ML+75ML SG</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>PERF. ESTUCHES HOMBRE</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2CC05963</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>INOPHARM RENU RECONSTRUCTING CHAMPU 250ML</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2CC05960</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>INOPHARM SCALP CARE ANTI-DANDRUFF CHAMPU 250ML</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2CC05961</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>INOPHARM SCALP CARE MICELLAR ANTI-DANDRUFF 250ML</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2CC05962</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>INOPHARM SCALP CARE REGROWTH CHAMPU 250ML</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>6XS18637</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>INOPHARM INTIMA EVERYDAY USE INTIMATE GEL 250ML</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>6XS18639</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>INOPHARM INTIMA EXTRA PROTECTION CARE 250ML</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>6XS18640</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>INOPHARM INTIMA INTIMATE GEL FEMENINE GUARD 250ML</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>6XS18641</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>INOPHARM INTIMA INTIMATE OIL MENOPAUSE 250ML</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2CA06703</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>INOPHARM RENU RECONSTRUCTING CONDITONER 250ML</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2CA06704</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>INOPHARM RENU RECONSTRUCTING HAIR MASK 250ML</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>